<commit_message>
AcidBee Enclosure - Door Hinge Dowell pins diameter clarification
Hinge Dowel Pins are 60mm by 5mm dia.
</commit_message>
<xml_diff>
--- a/bom/BOM_Enclosure_AcidBee.xlsx
+++ b/bom/BOM_Enclosure_AcidBee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{D9576D0A-9DB5-47F7-86FE-34BBB65B8FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA8894A-3826-4629-812C-4CF460CDC4F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D311E4F5-31DC-4B76-9478-1B05B30E6C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="135">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>M3X8_FlatHead_93395A201</t>
-  </si>
-  <si>
-    <t>Dowel Pin</t>
   </si>
   <si>
     <t>M5X3030_Twist in T Nut</t>
@@ -482,6 +479,12 @@
   </si>
   <si>
     <t>Nut, Roll in, M6</t>
+  </si>
+  <si>
+    <t>Dowel Pin 5mm Dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60mm Long X 5mm Diameter dowel pin. </t>
   </si>
 </sst>
 </file>
@@ -2939,9 +2942,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2979,9 +2982,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3014,26 +3017,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3066,26 +3052,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3261,25 +3230,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.453125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.453125" customWidth="1"/>
-    <col min="11" max="11" width="42.1796875" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" customWidth="1"/>
+    <col min="11" max="11" width="42.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3314,22 +3281,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>11</v>
@@ -3341,12 +3308,12 @@
       <c r="J2" s="11"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>13</v>
@@ -3368,15 +3335,15 @@
       <c r="J3" s="11"/>
       <c r="K3" s="17"/>
     </row>
-    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>17</v>
@@ -3394,21 +3361,21 @@
       <c r="J4" s="11"/>
       <c r="K4" s="17"/>
     </row>
-    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>11</v>
@@ -3420,15 +3387,15 @@
       <c r="J5" s="11"/>
       <c r="K5" s="17"/>
     </row>
-    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>20</v>
@@ -3446,15 +3413,15 @@
       <c r="J6" s="11"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>23</v>
@@ -3469,26 +3436,26 @@
         <v>20</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>11</v>
@@ -3496,25 +3463,27 @@
       <c r="H8" s="15">
         <v>8</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="16" t="s">
+        <v>134</v>
+      </c>
       <c r="J8" s="11"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>11</v>
@@ -3523,14 +3492,14 @@
         <v>1</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>11</v>
@@ -3539,10 +3508,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="21" t="s">
         <v>125</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>126</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>11</v>
@@ -3551,14 +3520,14 @@
         <v>4</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
@@ -3567,10 +3536,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>132</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>133</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>11</v>
@@ -3582,9 +3551,9 @@
       <c r="J11" s="19"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -3592,10 +3561,10 @@
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="15">
@@ -3603,25 +3572,25 @@
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="15">
@@ -3629,25 +3598,25 @@
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="15">
@@ -3655,25 +3624,25 @@
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="15">
@@ -3681,25 +3650,25 @@
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="15">
@@ -3707,15 +3676,15 @@
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11" t="s">
@@ -3723,10 +3692,10 @@
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="15">
@@ -3734,25 +3703,25 @@
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="15">
@@ -3760,190 +3729,190 @@
       </c>
       <c r="I18" s="16"/>
       <c r="J18" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="H19" s="15">
         <v>1</v>
       </c>
       <c r="I19" s="16"/>
       <c r="J19" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="15">
         <v>1</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>43</v>
-      </c>
       <c r="G21" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="15">
         <v>1</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>46</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="15">
         <v>1</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="15">
         <v>4</v>
       </c>
       <c r="I23" s="16"/>
       <c r="J23" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E24" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>51</v>
-      </c>
       <c r="G24" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="15">
         <v>1</v>
       </c>
       <c r="I24" s="16"/>
       <c r="J24" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="10"/>
@@ -3951,25 +3920,25 @@
         <v>6</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="10"/>
@@ -3978,22 +3947,22 @@
       </c>
       <c r="I26" s="16"/>
       <c r="J26" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="10"/>
@@ -4002,22 +3971,22 @@
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="10"/>
@@ -4025,25 +3994,25 @@
         <v>2</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="10"/>
@@ -4051,25 +4020,25 @@
         <v>2</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" s="14"/>
       <c r="G30" s="10"/>
@@ -4078,22 +4047,22 @@
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K30" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="10"/>
@@ -4102,25 +4071,25 @@
       </c>
       <c r="I31" s="16"/>
       <c r="J31" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K31" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="15">
@@ -4128,25 +4097,25 @@
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K32" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="15">
@@ -4154,55 +4123,55 @@
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K33" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H34" s="15">
         <v>1</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K34" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="15">
@@ -4210,137 +4179,137 @@
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K35" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H36" s="15">
         <v>1</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" s="10"/>
       <c r="C37" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H37" s="15">
         <v>1</v>
       </c>
       <c r="I37" s="16"/>
       <c r="J37" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K37" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="10"/>
       <c r="C38" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H38" s="15">
         <v>1</v>
       </c>
       <c r="I38" s="16"/>
       <c r="J38" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K38" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H39" s="15">
         <v>1</v>
       </c>
       <c r="I39" s="16"/>
       <c r="J39" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K39" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="15">
@@ -4348,25 +4317,25 @@
       </c>
       <c r="I40" s="16"/>
       <c r="J40" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K40" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="11" t="s">
         <v>28</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="15">
@@ -4374,25 +4343,25 @@
       </c>
       <c r="I41" s="16"/>
       <c r="J41" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K41" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" s="10"/>
       <c r="C42" s="11">
         <v>39</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="15">
@@ -4400,25 +4369,25 @@
       </c>
       <c r="I42" s="16"/>
       <c r="J42" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K42" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="11">
         <v>40</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G43" s="10"/>
       <c r="H43" s="15">
@@ -4426,25 +4395,25 @@
       </c>
       <c r="I43" s="16"/>
       <c r="J43" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K43" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B44" s="10"/>
       <c r="C44" s="11">
         <v>41</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G44" s="10"/>
       <c r="H44" s="15">
@@ -4452,25 +4421,25 @@
       </c>
       <c r="I44" s="16"/>
       <c r="J44" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K44" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="11">
         <v>42</v>
       </c>
       <c r="E45" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F45" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="15">
@@ -4478,10 +4447,10 @@
       </c>
       <c r="I45" s="16"/>
       <c r="J45" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K45" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4496,7 +4465,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
   <drawing r:id="rId6"/>
   <webPublishItems count="1">
-    <webPublishItem id="24158" divId="BOM_HextrudORT_Extruder_Dragon_24158" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_Enclosure_AcidBee.mht" autoRepublish="1"/>
+    <webPublishItem id="24158" divId="BOM_HextrudORT_Extruder_Dragon_24158" sourceType="sheet" destinationFile="C:\Users\olivi\HevORT\bom\BOM_Enclosure_AcidBee.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId7"/>

</xml_diff>

<commit_message>
Include Top lid Mod from Sillysam
Ref: https://discord.com/channels/790612368056647682/1206304279346942022/1206304279346942022
</commit_message>
<xml_diff>
--- a/bom/BOM_Enclosure_AcidBee.xlsx
+++ b/bom/BOM_Enclosure_AcidBee.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D311E4F5-31DC-4B76-9478-1B05B30E6C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1964782B-29B7-4E2D-A0B8-1A02F3C54847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="38560" windowHeight="21760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="172">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -350,9 +363,6 @@
   </si>
   <si>
     <t>Qty 2 due to Electronics Bay Hinge</t>
-  </si>
-  <si>
-    <t>2 per door.  2 front doors + elec bay door.</t>
   </si>
   <si>
     <t>PlateRH_Blank</t>
@@ -486,12 +496,141 @@
   <si>
     <t xml:space="preserve">60mm Long X 5mm Diameter dowel pin. </t>
   </si>
+  <si>
+    <t>Included in KIT</t>
+  </si>
+  <si>
+    <t>The Acid Bee enclosure offers a mean to keep the heat inside the chamber whith style. A The floating panel design that prevents undesired effect from material thermal expansion.  Magnetic latching doors and a top lid with gas struts.
+This design is meant for 3mm thick panel, but can easily be adapted to thicker materials.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HevORT Enclosure
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="36"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Acid Bee</t>
+    </r>
+  </si>
+  <si>
+    <t>M5X12_ButtonHeadScrew_91239A228</t>
+  </si>
+  <si>
+    <t>Screw, ButtonHead - M5X12mm</t>
+  </si>
+  <si>
+    <t>M4X8_CapScrew_91292A108</t>
+  </si>
+  <si>
+    <t>M4_Nut_94150A335</t>
+  </si>
+  <si>
+    <t>Nut, Hex - M4</t>
+  </si>
+  <si>
+    <t>GasStrut_Assembly</t>
+  </si>
+  <si>
+    <t>20 6inches Newton Gas Strut</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3uD51a2</t>
+  </si>
+  <si>
+    <t>Screw, Cap, M4X8mm</t>
+  </si>
+  <si>
+    <t>Qty 2 Due to Top Lid Hinge</t>
+  </si>
+  <si>
+    <t>Qty 3 due to Electronics Bay Hinge and Top Lid Hinge</t>
+  </si>
+  <si>
+    <t>2 per door.  2 front doors + elec bay door + Top Lid</t>
+  </si>
+  <si>
+    <t>BracketDoubler_Deco_LH</t>
+  </si>
+  <si>
+    <t>Bracket_Lid_LH</t>
+  </si>
+  <si>
+    <t>Bracket_Side</t>
+  </si>
+  <si>
+    <t>Handle Doubler_Lid (1)</t>
+  </si>
+  <si>
+    <t>Handle_Lid</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +745,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF00CCFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -615,9 +804,8 @@
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
+      <patternFill patternType="lightGrid">
+        <bgColor theme="1" tint="0.249977111117893"/>
       </patternFill>
     </fill>
   </fills>
@@ -627,41 +815,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -724,62 +877,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -794,6 +955,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -807,13 +1016,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -824,28 +1026,19 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
+        <sz val="14"/>
+        <color theme="6" tint="-0.249977111117893"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
           <color theme="0" tint="-0.499984740745262"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </right>
-        <top/>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -867,13 +1060,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149225</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1254505</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>1200195</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -911,13 +1104,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -955,13 +1148,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -999,13 +1192,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1043,13 +1236,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1087,13 +1280,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1131,13 +1324,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>212726</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>98426</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1311990</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1197690</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1175,13 +1368,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>92076</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1222119</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1140046</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1236,13 +1429,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>285751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1216025</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>1082088</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1297,13 +1490,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>136526</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>99851</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1177689</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1121817</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1358,13 +1551,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1237701</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1159266</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1419,13 +1612,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1463,13 +1656,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>117476</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>206375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1237498</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1198035</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1524,13 +1717,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155576</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>117476</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1254840</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>1216740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1568,13 +1761,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1612,13 +1805,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1656,13 +1849,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>174625</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>183332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1276730</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>1178231</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1717,13 +1910,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1761,13 +1954,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1805,13 +1998,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1849,13 +2042,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1893,13 +2086,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1937,13 +2130,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1981,13 +2174,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2025,13 +2218,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2069,13 +2262,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2113,13 +2306,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2157,13 +2350,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2201,13 +2394,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2245,13 +2438,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2289,13 +2482,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2333,13 +2526,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2377,13 +2570,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2421,13 +2614,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2465,13 +2658,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2509,13 +2702,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2553,13 +2746,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2597,13 +2790,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2641,13 +2834,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155575</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255174</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>1217074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2685,13 +2878,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>136526</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>187325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1197027</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>1182624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2746,13 +2939,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1314450</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1298047</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2790,13 +2983,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>209551</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1172400</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1263650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2834,13 +3027,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>188150</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>165101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1193800</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>1276350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2878,13 +3071,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>349251</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>215901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1174750</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1315720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2918,13 +3111,453 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>519546</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>265547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>935181</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>4064327</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BF2DC7A-42B4-FBCF-630B-3C678C2CFD07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="519546" y="265547"/>
+          <a:ext cx="3867726" cy="3798780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1381125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1262012</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="thumbnail_10.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3DA1D14-0307-48B0-B650-5ED6BFACFBBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3644900" y="8528050"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1374775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1325512</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="thumbnail_8.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD91C3A6-4B11-45CA-9B27-4C599FD7A775}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3638550" y="7156450"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1330325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1300112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="thumbnail_9.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8A3FE5F-EC8D-47BB-AD45-BB8DC4A40AA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3594100" y="8566150"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1355725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1300112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="thumbnail_2.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08F6986-3637-48AC-93F1-7981FD2C429B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3619500" y="7131050"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1311275</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>1287412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="thumbnail_17.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A706236-B855-4C8A-A771-35BEDCCB52A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3575050" y="74568050"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1311275</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1287412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="thumbnail_18.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53223D28-665A-4CA7-9B7A-78517936ECB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3575050" y="76003150"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1336675</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>1312812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="thumbnail_3.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EA95225-4523-4134-A482-5D6791091F49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="77463650"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1336675</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>1312812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="thumbnail_4.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21F8E018-3027-4297-9E4C-8FC8D5C39D2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="78898750"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1336675</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1312812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="thumbnail_5.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30AC58E6-F3C0-42C9-990A-8C6920689F1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3600450" y="80333850"/>
+          <a:ext cx="1190625" cy="1135012"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A1:K45" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2">
-  <autoFilter ref="A1:K45" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{494CDCE7-8EB1-486A-8076-EC1E59242533}" name="Table1" displayName="Table1" ref="A3:L56" totalsRowShown="0" headerRowBorderDxfId="3">
+  <autoFilter ref="A3:L56" xr:uid="{4DBD3307-5F20-47E0-9C75-3A8478E4F27D}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{8DD10BD1-F8F8-4CF0-8D4C-7F4FC801B3C7}" name="SubAssy"/>
     <tableColumn id="2" xr3:uid="{48F8A639-6252-46BC-8E09-3A18B47C9DCC}" name="Category"/>
     <tableColumn id="3" xr3:uid="{BE4DCEF1-3719-4618-878E-5276DFBA7F6C}" name="Item"/>
@@ -2933,6 +3566,7 @@
     <tableColumn id="6" xr3:uid="{873FF3B9-3553-41A7-82FD-A60CF1647DC7}" name="Part Description"/>
     <tableColumn id="7" xr3:uid="{0F03009E-09CE-4449-A2F4-75CD9645495C}" name="Make/Buy"/>
     <tableColumn id="8" xr3:uid="{3A8E6CB3-3EC7-4B91-88F5-471A655990CE}" name="QTY"/>
+    <tableColumn id="12" xr3:uid="{3995D13C-FFC2-4254-AACE-8B4E02079BC8}" name="Included in KIT" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{564A4095-287D-4969-92F8-291C82E276C5}" name="Comment"/>
     <tableColumn id="10" xr3:uid="{F8682D70-895E-48FC-9CE6-CE92B2E811DF}" name="Vendor" dataDxfId="1"/>
     <tableColumn id="11" xr3:uid="{5F238726-AAF1-402B-A03C-A7DC3685ED51}" name="Vendor URL" dataDxfId="0"/>
@@ -3228,1247 +3862,1815 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" customWidth="1"/>
-    <col min="11" max="11" width="42.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" customWidth="1"/>
+    <col min="10" max="10" width="76" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.453125" customWidth="1"/>
+    <col min="12" max="12" width="42.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="328.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="29" t="str">
+        <f>HYPERLINK("https://a360.co/49mWiYA","LINK TO CAD")</f>
+        <v>LINK TO CAD</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="27"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="92.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I3" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L3" s="22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="4" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H4" s="8">
+        <v>130</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="8">
+        <v>2</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="8">
+        <v>6</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="8">
+        <v>6</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="8">
+        <v>124</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="8">
+        <v>10</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="8">
+        <v>40</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="8">
+        <v>4</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="8">
+        <v>44</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="8">
+        <v>24</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="8">
+        <v>10</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="8">
+        <v>4</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="8">
+        <v>4</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="8">
+        <v>4</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L18" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="19" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="15">
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" s="8">
+        <v>8</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L19" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="17"/>
     </row>
-    <row r="4" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="20" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="15">
-        <v>30</v>
-      </c>
-      <c r="I4" s="16"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="17"/>
+      <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="8">
+        <v>24</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="21" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="15">
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="8">
+        <v>16</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="8">
+        <v>6</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="8">
         <v>4</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="17"/>
+      <c r="I23" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="24" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="15">
-        <v>30</v>
-      </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="17"/>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H24" s="8">
+        <v>26</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="25" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="15">
-        <v>20</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="17"/>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L25" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="26" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="B26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="8">
+        <v>1</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L26" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="15">
+    </row>
+    <row r="27" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H27" s="8">
+        <v>1</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="8">
+        <v>1</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="8">
+        <v>5</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="8">
+        <v>1</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J30" s="9"/>
+      <c r="K30" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="8">
         <v>8</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="17"/>
+      <c r="I31" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="32" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="15">
+      <c r="B32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="8">
         <v>1</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="17"/>
+      <c r="I32" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="33" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="11">
+      <c r="B33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="8">
+        <v>2</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L33" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="8">
+        <v>2</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="8">
+        <v>3</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H36" s="8">
         <v>4</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="15">
+      <c r="I36" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J36" s="9"/>
+      <c r="K36" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="8">
         <v>4</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I37" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J37" s="9"/>
+      <c r="K37" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J38" s="9"/>
+      <c r="K38" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J39" s="9"/>
+      <c r="K39" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L39" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L40" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="8">
+        <v>1</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J41" s="9"/>
+      <c r="K41" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L41" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="8">
+        <v>1</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J42" s="9"/>
+      <c r="K42" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L42" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H43" s="8">
+        <v>1</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J43" s="9"/>
+      <c r="K43" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L43" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H44" s="8">
+        <v>1</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J44" s="9"/>
+      <c r="K44" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L44" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H45" s="8">
+        <v>1</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J45" s="9"/>
+      <c r="K45" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L45" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H46" s="8">
+        <v>2</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J46" s="9"/>
+      <c r="K46" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L46" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H47" s="8">
+        <v>2</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J47" s="9"/>
+      <c r="K47" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L47" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
+      <c r="F48" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H48" s="8">
+        <v>1</v>
+      </c>
+      <c r="I48" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J48" s="9"/>
+      <c r="K48" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L48" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="49" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="11">
-        <v>4</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="15">
-        <v>4</v>
-      </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
+      <c r="B49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" s="8">
+        <v>1</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J49" s="9"/>
+      <c r="K49" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="L49" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="50" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="15">
-        <v>4</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K12" s="18" t="s">
+      <c r="B50" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" s="8">
+        <v>1</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J50" s="9"/>
+      <c r="K50" s="11" t="s">
         <v>121</v>
       </c>
+      <c r="L50" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="51" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="15">
-        <v>8</v>
-      </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K13" s="18" t="s">
+      <c r="B51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H51" s="8">
+        <v>1</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J51" s="9"/>
+      <c r="K51" s="11" t="s">
         <v>121</v>
       </c>
+      <c r="L51" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="52" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="15">
-        <v>24</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K14" s="18" t="s">
+      <c r="B52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H52" s="8">
+        <v>1</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J52" s="9"/>
+      <c r="K52" s="11" t="s">
         <v>121</v>
       </c>
+      <c r="L52" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="53" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="15">
-        <v>16</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K15" s="18" t="s">
+      <c r="B53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53" s="8">
+        <v>1</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J53" s="9"/>
+      <c r="K53" s="11" t="s">
         <v>121</v>
       </c>
+      <c r="L53" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="54" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="15">
-        <v>6</v>
-      </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K16" s="18" t="s">
+      <c r="B54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H54" s="8">
+        <v>2</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J54" s="9"/>
+      <c r="K54" s="11" t="s">
         <v>121</v>
       </c>
+      <c r="L54" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="55" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="15">
-        <v>4</v>
-      </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K17" s="18" t="s">
+      <c r="B55" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H55" s="8">
+        <v>2</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J55" s="9"/>
+      <c r="K55" s="11" t="s">
         <v>121</v>
       </c>
+      <c r="L55" s="11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="56" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="15">
-        <v>26</v>
-      </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K18" s="18" t="s">
+      <c r="B56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H56" s="8">
+        <v>2</v>
+      </c>
+      <c r="I56" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="J56" s="9"/>
+      <c r="K56" s="11" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="15">
-        <v>1</v>
-      </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="15">
-        <v>1</v>
-      </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="15">
-        <v>1</v>
-      </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K21" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H22" s="15">
-        <v>1</v>
-      </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H23" s="15">
-        <v>4</v>
-      </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="15">
-        <v>1</v>
-      </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="15">
-        <v>6</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="J25" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K25" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="15">
-        <v>1</v>
-      </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="15">
-        <v>1</v>
-      </c>
-      <c r="I27" s="16"/>
-      <c r="J27" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="15">
-        <v>2</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K28" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="15">
-        <v>2</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="15">
-        <v>3</v>
-      </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="15">
-        <v>3</v>
-      </c>
-      <c r="I31" s="16"/>
-      <c r="J31" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K31" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="10"/>
-      <c r="H32" s="15">
-        <v>1</v>
-      </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K32" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="15">
-        <v>1</v>
-      </c>
-      <c r="I33" s="16"/>
-      <c r="J33" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K33" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H34" s="15">
-        <v>1</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="15">
-        <v>1</v>
-      </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H36" s="15">
-        <v>1</v>
-      </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H37" s="15">
-        <v>1</v>
-      </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K37" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H38" s="15">
-        <v>1</v>
-      </c>
-      <c r="I38" s="16"/>
-      <c r="J38" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H39" s="15">
-        <v>1</v>
-      </c>
-      <c r="I39" s="16"/>
-      <c r="J39" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K39" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="15">
-        <v>2</v>
-      </c>
-      <c r="I40" s="16"/>
-      <c r="J40" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="15">
-        <v>2</v>
-      </c>
-      <c r="I41" s="16"/>
-      <c r="J41" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K41" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="11">
-        <v>39</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="15">
-        <v>1</v>
-      </c>
-      <c r="I42" s="16"/>
-      <c r="J42" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11">
-        <v>40</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="15">
-        <v>1</v>
-      </c>
-      <c r="I43" s="16"/>
-      <c r="J43" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="11">
-        <v>41</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G44" s="10"/>
-      <c r="H44" s="15">
-        <v>1</v>
-      </c>
-      <c r="I44" s="16"/>
-      <c r="J44" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K44" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="11">
-        <v>42</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G45" s="10"/>
-      <c r="H45" s="15">
-        <v>1</v>
-      </c>
-      <c r="I45" s="16"/>
-      <c r="J45" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>121</v>
+      <c r="L56" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K12" r:id="rId1" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{D59588BB-D693-4E5D-A874-744FF7A5C2DE}"/>
-    <hyperlink ref="J12" r:id="rId2" display="https://www.thingiverse.com/thing:5188673" xr:uid="{1F2091BC-041A-4A27-BAC7-8A408EEBE19D}"/>
-    <hyperlink ref="K13:K45" r:id="rId3" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{41DC48DE-AFC0-44A5-8DBF-FF5C3804786A}"/>
-    <hyperlink ref="J13:J45" r:id="rId4" display="https://www.thingiverse.com/thing:5188673" xr:uid="{64B4F3F8-DA2F-4B10-A68A-FD27B6C892B8}"/>
+    <hyperlink ref="L18" r:id="rId1" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{D59588BB-D693-4E5D-A874-744FF7A5C2DE}"/>
+    <hyperlink ref="K18" r:id="rId2" display="https://www.thingiverse.com/thing:5188673" xr:uid="{1F2091BC-041A-4A27-BAC7-8A408EEBE19D}"/>
+    <hyperlink ref="L19:L51" r:id="rId3" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{41DC48DE-AFC0-44A5-8DBF-FF5C3804786A}"/>
+    <hyperlink ref="K19:K51" r:id="rId4" display="https://www.thingiverse.com/thing:5188673" xr:uid="{64B4F3F8-DA2F-4B10-A68A-FD27B6C892B8}"/>
+    <hyperlink ref="L52" r:id="rId5" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{49CAF032-F0FA-47F5-893F-163C284BFC43}"/>
+    <hyperlink ref="L53" r:id="rId6" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{5C69A10E-935D-47F4-AB12-F2612F6BF5BE}"/>
+    <hyperlink ref="L54" r:id="rId7" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{E80C4321-3298-420E-9740-50211831F36C}"/>
+    <hyperlink ref="L55" r:id="rId8" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{9EB6511B-9DDB-4913-A8E7-F1822ECE9425}"/>
+    <hyperlink ref="L56" r:id="rId9" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/Enclosure/AcidBee_Enclosure" xr:uid="{346D9482-4B49-4732-8C55-B4391FDAB495}"/>
+    <hyperlink ref="K52" r:id="rId10" display="https://www.thingiverse.com/thing:5188673" xr:uid="{2A27946F-D8BB-4832-BBE5-89A2C06339C9}"/>
+    <hyperlink ref="K53" r:id="rId11" display="https://www.thingiverse.com/thing:5188673" xr:uid="{B6510B45-69D2-4A55-B8C3-22583968FDEB}"/>
+    <hyperlink ref="K54" r:id="rId12" display="https://www.thingiverse.com/thing:5188673" xr:uid="{75719AF2-339E-4150-838A-50EBAF09B65A}"/>
+    <hyperlink ref="K55" r:id="rId13" display="https://www.thingiverse.com/thing:5188673" xr:uid="{6F3D217F-EFD5-4796-8ED2-588C897F450E}"/>
+    <hyperlink ref="K56" r:id="rId14" display="https://www.thingiverse.com/thing:5188673" xr:uid="{D23F6CAF-9E6B-4951-BD3E-7EE0EF59D786}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
+  <drawing r:id="rId16"/>
   <webPublishItems count="1">
     <webPublishItem id="24158" divId="BOM_HextrudORT_Extruder_Dragon_24158" sourceType="sheet" destinationFile="C:\Users\olivi\HevORT\bom\BOM_Enclosure_AcidBee.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>